<commit_message>
Small documentation updates: fixed typos and small text improvements
</commit_message>
<xml_diff>
--- a/Documentation/Documents/CRC-карты.xlsx
+++ b/Documentation/Documents/CRC-карты.xlsx
@@ -48,10 +48,10 @@
     <t>Получение случайного значения из словаря - выбираем случайного значение из ассоциативного массива без учета его ключей</t>
   </si>
   <si>
-    <t>Расширяет .NET класс Dictionary указанными методами. Влияет на все Dictionary, которые используют пространство имен, где находится этот класс</t>
-  </si>
-  <si>
     <t>Методы расширения использует класс Gameplay для создания случайного противника</t>
+  </si>
+  <si>
+    <t>Расширяет .NET класс Dictionary указанными методами. Влияет на все Dictionary, которые используют пространство имен, этого класса</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,13 +616,13 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I17" s="9"/>
     </row>

</xml_diff>